<commit_message>
Changes in Invpoice Generator Page
</commit_message>
<xml_diff>
--- a/InvoiceLogTemplate.xlsx
+++ b/InvoiceLogTemplate.xlsx
@@ -762,7 +762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1952,6 +1952,38 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Ali</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">machine </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Ali</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>streamlit</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>